<commit_message>
tried a color wheel scheme calculated from HSL with perfect angle spacing and it looked terrible.  Went back to hand-jammed.
</commit_message>
<xml_diff>
--- a/Final Project/RGB_Colors.xlsx
+++ b/Final Project/RGB_Colors.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
   <si>
     <t>R</t>
   </si>
@@ -34,6 +34,42 @@
   </si>
   <si>
     <t>RGB</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Perfect</t>
+  </si>
+  <si>
+    <t>Spacing</t>
+  </si>
+  <si>
+    <t>Looks</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>Hand</t>
+  </si>
+  <si>
+    <t>Adjusted</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>&lt;---</t>
+  </si>
+  <si>
+    <t>---&gt;</t>
   </si>
 </sst>
 </file>
@@ -77,9 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -381,15 +418,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21:H36"/>
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -402,14 +439,17 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="F1">
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1">
         <v>20</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -422,20 +462,23 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <f>B2*$F$1</f>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2">
+        <f>B2*$G$1</f>
         <v>200</v>
       </c>
-      <c r="G2">
-        <f t="shared" ref="G2:H2" si="0">C2*$F$1</f>
-        <v>0</v>
-      </c>
       <c r="H2">
+        <f t="shared" ref="H2:I2" si="0">C2*$G$1</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -448,20 +491,23 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F17" si="1">B3*$F$1</f>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G17" si="1">B3*$G$1</f>
         <v>200</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G17" si="2">C3*$F$1</f>
-        <v>0</v>
-      </c>
       <c r="H3">
-        <f t="shared" ref="H3:H17" si="3">D3*$F$1</f>
+        <f t="shared" ref="H3:H17" si="2">C3*$G$1</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I17" si="3">D3*$G$1</f>
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -474,20 +520,23 @@
       <c r="D4">
         <v>5</v>
       </c>
-      <c r="F4">
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -500,20 +549,23 @@
       <c r="D5">
         <v>7</v>
       </c>
-      <c r="F5">
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <f t="shared" si="3"/>
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -526,20 +578,20 @@
       <c r="D6">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -552,20 +604,20 @@
       <c r="D7">
         <v>12</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <f t="shared" si="3"/>
         <v>240</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -578,20 +630,20 @@
       <c r="D8">
         <v>8</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <f t="shared" si="3"/>
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -604,20 +656,20 @@
       <c r="D9">
         <v>3</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -630,20 +682,20 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -656,20 +708,20 @@
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -682,20 +734,20 @@
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -708,20 +760,20 @@
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -734,20 +786,20 @@
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -760,20 +812,20 @@
       <c r="D15">
         <v>0</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <f t="shared" si="1"/>
         <v>160</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -786,20 +838,20 @@
       <c r="D16">
         <v>0</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -812,20 +864,20 @@
       <c r="D17">
         <v>0</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
@@ -838,14 +890,38 @@
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="F20">
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20">
         <v>20</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K20" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" t="s">
+        <v>6</v>
+      </c>
+      <c r="M20" t="s">
+        <v>7</v>
+      </c>
+      <c r="N20" t="s">
+        <v>8</v>
+      </c>
+      <c r="P20" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>1</v>
+      </c>
+      <c r="R20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0</v>
       </c>
@@ -858,20 +934,44 @@
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="F21">
-        <f>B21*$F$20</f>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21">
+        <f>B21*$G$20</f>
         <v>200</v>
       </c>
-      <c r="G21">
-        <f t="shared" ref="G21:H21" si="4">C21*$F$20</f>
-        <v>0</v>
-      </c>
       <c r="H21">
+        <f t="shared" ref="H21:I21" si="4">C21*$G$20</f>
+        <v>0</v>
+      </c>
+      <c r="I21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K21" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>100</v>
+      </c>
+      <c r="N21">
+        <v>50</v>
+      </c>
+      <c r="P21">
+        <v>255</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -884,20 +984,44 @@
       <c r="D22">
         <v>1</v>
       </c>
-      <c r="F22">
-        <f t="shared" ref="F22:F36" si="5">B22*$F$20</f>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:G36" si="5">B22*$G$20</f>
         <v>200</v>
       </c>
-      <c r="G22">
-        <f t="shared" ref="G22:G36" si="6">C22*$F$20</f>
-        <v>0</v>
-      </c>
       <c r="H22">
-        <f t="shared" ref="H22:H36" si="7">D22*$F$20</f>
+        <f t="shared" ref="H22:H36" si="6">C22*$G$20</f>
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ref="I22:I36" si="7">D22*$G$20</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K22" t="s">
+        <v>11</v>
+      </c>
+      <c r="L22">
+        <v>22</v>
+      </c>
+      <c r="M22">
+        <v>100</v>
+      </c>
+      <c r="N22">
+        <v>50</v>
+      </c>
+      <c r="P22">
+        <v>255</v>
+      </c>
+      <c r="Q22">
+        <v>94</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
@@ -910,20 +1034,44 @@
       <c r="D23">
         <v>5</v>
       </c>
-      <c r="F23">
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <f t="shared" si="7"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23">
+        <v>45</v>
+      </c>
+      <c r="M23">
+        <v>100</v>
+      </c>
+      <c r="N23">
+        <v>50</v>
+      </c>
+      <c r="P23">
+        <v>255</v>
+      </c>
+      <c r="Q23">
+        <v>191</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3</v>
       </c>
@@ -936,20 +1084,44 @@
       <c r="D24">
         <v>7</v>
       </c>
-      <c r="F24">
+      <c r="E24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <f t="shared" si="7"/>
         <v>140</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24">
+        <v>67</v>
+      </c>
+      <c r="M24">
+        <v>100</v>
+      </c>
+      <c r="N24">
+        <v>50</v>
+      </c>
+      <c r="P24">
+        <v>225</v>
+      </c>
+      <c r="Q24">
+        <v>255</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>4</v>
       </c>
@@ -962,20 +1134,38 @@
       <c r="D25">
         <v>10</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <f t="shared" si="7"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L25">
+        <v>90</v>
+      </c>
+      <c r="M25">
+        <v>100</v>
+      </c>
+      <c r="N25">
+        <v>50</v>
+      </c>
+      <c r="P25">
+        <v>128</v>
+      </c>
+      <c r="Q25">
+        <v>255</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>5</v>
       </c>
@@ -988,20 +1178,38 @@
       <c r="D26">
         <v>12</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <f t="shared" si="7"/>
         <v>240</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L26">
+        <v>112</v>
+      </c>
+      <c r="M26">
+        <v>100</v>
+      </c>
+      <c r="N26">
+        <v>50</v>
+      </c>
+      <c r="P26">
+        <v>34</v>
+      </c>
+      <c r="Q26">
+        <v>255</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>6</v>
       </c>
@@ -1014,20 +1222,38 @@
       <c r="D27">
         <v>10</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <f t="shared" si="7"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L27">
+        <v>135</v>
+      </c>
+      <c r="M27">
+        <v>100</v>
+      </c>
+      <c r="N27">
+        <v>50</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>255</v>
+      </c>
+      <c r="R27">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>7</v>
       </c>
@@ -1040,20 +1266,38 @@
       <c r="D28">
         <v>8</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <f t="shared" si="7"/>
         <v>160</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L28">
+        <v>157</v>
+      </c>
+      <c r="M28">
+        <v>100</v>
+      </c>
+      <c r="N28">
+        <v>50</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="Q28">
+        <v>255</v>
+      </c>
+      <c r="R28">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>8</v>
       </c>
@@ -1066,20 +1310,38 @@
       <c r="D29">
         <v>5</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <f t="shared" si="6"/>
         <v>80</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <f t="shared" si="7"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L29">
+        <v>180</v>
+      </c>
+      <c r="M29">
+        <v>100</v>
+      </c>
+      <c r="N29">
+        <v>50</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+      <c r="Q29">
+        <v>255</v>
+      </c>
+      <c r="R29">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>9</v>
       </c>
@@ -1092,20 +1354,38 @@
       <c r="D30">
         <v>4</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <f t="shared" si="6"/>
         <v>120</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <f t="shared" si="7"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L30">
+        <v>202</v>
+      </c>
+      <c r="M30">
+        <v>100</v>
+      </c>
+      <c r="N30">
+        <v>50</v>
+      </c>
+      <c r="P30">
+        <v>0</v>
+      </c>
+      <c r="Q30">
+        <v>162</v>
+      </c>
+      <c r="R30">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>10</v>
       </c>
@@ -1118,20 +1398,38 @@
       <c r="D31">
         <v>2</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <f t="shared" si="6"/>
         <v>160</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <f t="shared" si="7"/>
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L31">
+        <v>225</v>
+      </c>
+      <c r="M31">
+        <v>100</v>
+      </c>
+      <c r="N31">
+        <v>50</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>64</v>
+      </c>
+      <c r="R31">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>11</v>
       </c>
@@ -1144,20 +1442,38 @@
       <c r="D32">
         <v>0</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <f t="shared" si="6"/>
         <v>200</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L32">
+        <v>247</v>
+      </c>
+      <c r="M32">
+        <v>100</v>
+      </c>
+      <c r="N32">
+        <v>50</v>
+      </c>
+      <c r="P32">
+        <v>30</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>12</v>
       </c>
@@ -1170,20 +1486,38 @@
       <c r="D33">
         <v>0</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <f t="shared" si="6"/>
         <v>140</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L33">
+        <v>270</v>
+      </c>
+      <c r="M33">
+        <v>100</v>
+      </c>
+      <c r="N33">
+        <v>50</v>
+      </c>
+      <c r="P33">
+        <v>128</v>
+      </c>
+      <c r="Q33">
+        <v>0</v>
+      </c>
+      <c r="R33">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>13</v>
       </c>
@@ -1196,20 +1530,38 @@
       <c r="D34">
         <v>0</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <f t="shared" si="5"/>
         <v>100</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L34">
+        <v>292</v>
+      </c>
+      <c r="M34">
+        <v>100</v>
+      </c>
+      <c r="N34">
+        <v>50</v>
+      </c>
+      <c r="P34">
+        <v>221</v>
+      </c>
+      <c r="Q34">
+        <v>0</v>
+      </c>
+      <c r="R34">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>14</v>
       </c>
@@ -1222,20 +1574,38 @@
       <c r="D35">
         <v>0</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <f t="shared" si="5"/>
         <v>140</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L35">
+        <v>315</v>
+      </c>
+      <c r="M35">
+        <v>100</v>
+      </c>
+      <c r="N35">
+        <v>50</v>
+      </c>
+      <c r="P35">
+        <v>255</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>15</v>
       </c>
@@ -1248,17 +1618,35 @@
       <c r="D36">
         <v>0</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <f t="shared" si="5"/>
         <v>180</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <f t="shared" si="7"/>
         <v>0</v>
+      </c>
+      <c r="L36">
+        <v>337</v>
+      </c>
+      <c r="M36">
+        <v>100</v>
+      </c>
+      <c r="N36">
+        <v>50</v>
+      </c>
+      <c r="P36">
+        <v>255</v>
+      </c>
+      <c r="Q36">
+        <v>0</v>
+      </c>
+      <c r="R36">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>